<commit_message>
complete 5th data addded with export csv
</commit_message>
<xml_diff>
--- a/public/files/3_mar.xlsx
+++ b/public/files/3_mar.xlsx
@@ -2900,10 +2900,10 @@
         <v>15</v>
       </c>
       <c r="F60" s="5">
-        <v>86435.0</v>
+        <v>35.0</v>
       </c>
       <c r="G60" s="5">
-        <v>1440.58333333333</v>
+        <v>0.583333</v>
       </c>
       <c r="H60" s="5" t="s">
         <v>95</v>

</xml_diff>